<commit_message>
update from gridea: 2021-11-14 10:32:37
</commit_message>
<xml_diff>
--- a/lifeRestart/data/talents.xlsx
+++ b/lifeRestart/data/talents.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84694\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84694\Desktop\人生重来\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F33440-1349-49EC-8228-3642668C2CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC5D45B-00AC-4951-8246-510F02069F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="talents" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="473">
   <si>
     <t>序号</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -522,530 +522,514 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>天龙人</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你拥有北京户口</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>独生子女</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你没有兄弟姐妹</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>乡间微风</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你出生在农村</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你出生在城市</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>城中高楼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你有美国国籍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>美籍华人</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>家中老大</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你最受父母宠爱</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水性良好</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不会被淹死</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>先天免疫</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你不会得艾滋病</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有属性+1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>额外家境</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>额外颜值</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>额外体质</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>额外智力</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>额外快乐</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>快乐+1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>快乐-3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>快乐+2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>超凡</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>父母美貌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>颜值+2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>红颜薄命</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>颜值+2，体质-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>属蛇</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不会被蛇咬死</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有属性+2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>半神</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>人中龙凤</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>天生双重性别</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>阴阳之外</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>天生无性别</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斩情证道</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>终生不恋爱结婚</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>桃花连连</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>12岁前父母都健在</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>平安童年</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>宠物大师</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>宠物不会意外死亡</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>天生残疾</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>体质-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>早产儿</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有属性-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>体质-10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>十死无生</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>家运不顺</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>家境-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>头着地</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>智力-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>胎教</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>智力+1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>班中红人</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>和同学容易处好关系</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>骑士</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>能轻松学会骑车</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>永远的神</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>电竞天才</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>可能和同性交往</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>彩虹之下</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>丁克</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>赌毒不沾</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不生孩子</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>少数民族</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>高考+5分</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>恋爱机会提升</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>老司机</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你的家人不会心脏病</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>低压</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战功</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你退伍后会当官</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不孕不育</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你生不出孩子</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>白头偕老</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>爱人至少能活到70岁</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>100岁时才能开启</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>effect:SPR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>effect:MNY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>effect:CHR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>effect:STR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>effect:INT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>三十而立</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>四十不惑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>30岁时家境+2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>40岁时智力+2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>知天命</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>50岁时智力、快乐+1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>耳顺</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>60岁时快乐+2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>从心所欲</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>70岁时快乐+3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>老当益壮</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>60岁时体质+2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>鹤发童颜</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>70岁时颜值+3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>学前启蒙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5岁时智力+2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>十八变</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>18岁时颜值+2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>迟来之财</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>90岁时家境+4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>condition</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发条件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>理财达人</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>成熟</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>形象管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>成年礼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>18岁时快乐+1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始可用属性点+1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始可用属性点+8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始可用属性点+4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>天命</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>人类进化</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>开光之胎</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>祖传药丸</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>神秘的小盒子</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能不明</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>家境为0时家境+1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>乐天派</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>天龙人</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>你拥有北京户口</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>独生子女</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>你没有兄弟姐妹</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>乡间微风</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>你出生在农村</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>你出生在城市</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>城中高楼</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>你有美国国籍</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>美籍华人</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>家中老大</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>你最受父母宠爱</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>水性良好</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>不会被淹死</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>先天免疫</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>你不会得艾滋病</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有属性+1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>额外家境</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>额外颜值</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>额外体质</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>额外智力</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>额外快乐</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>快乐+1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>快乐-3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>快乐+2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>超凡</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>父母美貌</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>颜值+2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>红颜薄命</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>颜值+2，体质-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>属蛇</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>不会被蛇咬死</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有属性+2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>半神</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>人中龙凤</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>天生双重性别</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>阴阳之外</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>天生无性别</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>斩情证道</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>终生不恋爱结婚</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>桃花连连</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>12岁前父母都健在</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>平安童年</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>宠物大师</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>宠物不会意外死亡</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>天生残疾</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>体质-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>早产儿</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有属性-1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>体质-10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>十死无生</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>家运不顺</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>家境-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>头着地</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>智力-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>胎教</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>智力+1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>班中红人</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>和同学容易处好关系</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>骑士</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>能轻松学会骑车</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>永远的神</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>电竞天才</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>可能和同性交往</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>彩虹之下</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>丁克</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>赌毒不沾</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>不生孩子</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>少数民族</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>高考+5分</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>恋爱机会提升</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>老司机</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>你的家人不会心脏病</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>低压</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>战功</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>你退伍后会当官</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>不孕不育</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>你生不出孩子</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>白头偕老</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>爱人至少能活到70岁</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>100岁时才能开启</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>$id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>effect:SPR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>effect:MNY</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>effect:CHR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>effect:STR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>effect:INT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>三十而立</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>四十不惑</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>30岁时家境+2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>40岁时智力+2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>知天命</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>50岁时智力、快乐+1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>耳顺</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>60岁时快乐+2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>从心所欲</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>70岁时快乐+3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>老当益壮</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>60岁时体质+2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>鹤发童颜</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>70岁时颜值+3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>学前启蒙</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>5岁时智力+2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>十八变</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>18岁时颜值+2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>迟来之财</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>90岁时家境+4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>condition</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>触发条件</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>理财达人</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>30、40、50岁时家境+1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>成熟</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>12、18岁时智力+1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>形象管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>16、24岁时颜值+1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>成年礼</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>18岁时快乐+1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始可用属性点+1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始可用属性点+8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始可用属性点+4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>天命</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>人类进化</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>开光之胎</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>祖传药丸</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>神秘的小盒子</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>功能不明</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>家境为0时家境+1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>乐天派</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>快乐为0时快乐+1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1110,15 +1094,6 @@
     <t>AGE?[90]</t>
   </si>
   <si>
-    <t>AGE?[30,40,50]</t>
-  </si>
-  <si>
-    <t>AGE?[12,18]</t>
-  </si>
-  <si>
-    <t>AGE?[16,24]</t>
-  </si>
-  <si>
     <t>(AGE?[20])&amp;(INT&gt;8)</t>
   </si>
   <si>
@@ -1312,10 +1287,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>体质&lt;-1时其他属性+2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>活死人</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1815,6 +1786,62 @@
   </si>
   <si>
     <t>不知道有什么用……</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>返老还童</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>可能会回到年轻的时候</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>时光倒流</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>或许时间会倒流</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>转世重修</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>渡劫失败重生</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGE?[40]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>40岁时家境+3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>18岁时智力+2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGE?[18]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>24岁时颜值+2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGE?[24]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>体质&lt;0时其他属性+2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>乐观</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2219,13 +2246,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q133"/>
+  <dimension ref="A1:Q136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D129" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C135" sqref="C135"/>
+      <selection pane="bottomRight" activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.44140625" defaultRowHeight="39.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2246,55 +2273,55 @@
   <sheetData>
     <row r="1" spans="1:17" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="L1" s="7" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2308,7 +2335,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -2317,37 +2344,37 @@
         <v>7</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="L2" s="8" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2358,7 +2385,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -2372,7 +2399,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -2395,10 +2422,10 @@
         <v>11</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="O5" s="1">
         <v>1113</v>
@@ -2418,13 +2445,13 @@
         <v>1</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2446,10 +2473,10 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>136</v>
+        <v>472</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -2483,7 +2510,7 @@
         <v>135</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -2500,7 +2527,7 @@
         <v>131</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -2514,22 +2541,22 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="E12" s="1">
         <v>2</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2537,10 +2564,10 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -2551,22 +2578,22 @@
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="E14" s="1">
         <v>0</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2574,22 +2601,22 @@
         <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2597,10 +2624,10 @@
         <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
@@ -2609,13 +2636,13 @@
         <v>3</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2623,10 +2650,10 @@
         <v>27</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -2637,10 +2664,10 @@
         <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -2651,10 +2678,10 @@
         <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -2665,10 +2692,10 @@
         <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
@@ -2694,10 +2721,10 @@
         <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
@@ -2711,10 +2738,10 @@
         <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -2728,10 +2755,10 @@
         <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
@@ -2748,10 +2775,10 @@
         <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -2762,10 +2789,10 @@
         <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E25" s="1">
         <v>3</v>
@@ -2791,22 +2818,22 @@
         <v>36</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="E26" s="1">
         <v>2</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="M26" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2814,19 +2841,19 @@
         <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="E27" s="1">
         <v>2</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="N27" s="6" t="s">
         <v>11</v>
@@ -2840,16 +2867,16 @@
         <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2857,16 +2884,16 @@
         <v>39</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="E29" s="1">
         <v>1</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2874,10 +2901,10 @@
         <v>40</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -2888,10 +2915,10 @@
         <v>41</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -2902,10 +2929,10 @@
         <v>42</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -2916,10 +2943,10 @@
         <v>43</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
@@ -2933,10 +2960,10 @@
         <v>44</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -2962,10 +2989,10 @@
         <v>45</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
@@ -2979,10 +3006,10 @@
         <v>46</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
@@ -2996,10 +3023,10 @@
         <v>47</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -3013,10 +3040,10 @@
         <v>48</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -3030,10 +3057,10 @@
         <v>49</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
@@ -3044,10 +3071,10 @@
         <v>50</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
@@ -3058,10 +3085,10 @@
         <v>51</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -3072,10 +3099,10 @@
         <v>52</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
@@ -3086,16 +3113,16 @@
         <v>53</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3103,10 +3130,10 @@
         <v>54</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
@@ -3117,10 +3144,10 @@
         <v>55</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
@@ -3131,10 +3158,10 @@
         <v>56</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -3145,10 +3172,10 @@
         <v>57</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
@@ -3159,16 +3186,16 @@
         <v>58</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="E48" s="1">
         <v>1</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3176,10 +3203,10 @@
         <v>59</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="E49" s="1">
         <v>1</v>
@@ -3190,10 +3217,10 @@
         <v>60</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E50" s="1">
         <v>3</v>
@@ -3204,13 +3231,13 @@
         <v>61</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -3224,13 +3251,13 @@
         <v>62</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
@@ -3244,13 +3271,13 @@
         <v>63</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="D53" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -3267,13 +3294,13 @@
         <v>64</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="D54" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
@@ -3287,13 +3314,13 @@
         <v>65</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="D55" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
@@ -3307,13 +3334,13 @@
         <v>66</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="D56" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E56" s="1">
         <v>1</v>
@@ -3327,13 +3354,13 @@
         <v>67</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>239</v>
-      </c>
       <c r="D57" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -3347,13 +3374,13 @@
         <v>68</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="D58" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E58" s="1">
         <v>1</v>
@@ -3367,13 +3394,13 @@
         <v>69</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="D59" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E59" s="1">
         <v>1</v>
@@ -3387,13 +3414,13 @@
         <v>70</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>245</v>
-      </c>
       <c r="D60" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E60" s="1">
         <v>0</v>
@@ -3407,19 +3434,19 @@
         <v>71</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>249</v>
+        <v>466</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>285</v>
+        <v>465</v>
       </c>
       <c r="E61" s="1">
         <v>0</v>
       </c>
       <c r="H61" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3427,19 +3454,19 @@
         <v>72</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>251</v>
+        <v>467</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>286</v>
+        <v>468</v>
       </c>
       <c r="E62" s="1">
         <v>1</v>
       </c>
       <c r="K62" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3447,19 +3474,19 @@
         <v>73</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>253</v>
+        <v>469</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>287</v>
+        <v>470</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
       </c>
       <c r="I63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3467,13 +3494,13 @@
         <v>74</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E64" s="1">
         <v>0</v>
@@ -3487,10 +3514,10 @@
         <v>75</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E65" s="1">
         <v>0</v>
@@ -3504,10 +3531,10 @@
         <v>76</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E66" s="1">
         <v>3</v>
@@ -3521,10 +3548,10 @@
         <v>77</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E67" s="1">
         <v>1</v>
@@ -3535,13 +3562,13 @@
         <v>78</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="E68" s="1">
         <v>0</v>
@@ -3555,13 +3582,13 @@
         <v>79</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="E69" s="1">
         <v>1</v>
@@ -3575,13 +3602,13 @@
         <v>80</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="E70" s="1">
         <v>0</v>
@@ -3595,13 +3622,13 @@
         <v>81</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="E71" s="1">
         <v>0</v>
@@ -3615,13 +3642,13 @@
         <v>82</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="E72" s="1">
         <v>0</v>
@@ -3635,10 +3662,10 @@
         <v>83</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E73" s="1">
         <v>0</v>
@@ -3649,10 +3676,10 @@
         <v>84</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E74" s="1">
         <v>0</v>
@@ -3663,10 +3690,10 @@
         <v>85</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="E75" s="1">
         <v>0</v>
@@ -3677,13 +3704,13 @@
         <v>86</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E76" s="1">
         <v>1</v>
@@ -3697,13 +3724,13 @@
         <v>87</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="E77" s="1">
         <v>0</v>
@@ -3717,13 +3744,13 @@
         <v>88</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="E78" s="1">
         <v>1</v>
@@ -3737,13 +3764,13 @@
         <v>89</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="E79" s="1">
         <v>1</v>
@@ -3757,13 +3784,13 @@
         <v>90</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E80" s="1">
         <v>0</v>
@@ -3777,13 +3804,13 @@
         <v>91</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E81" s="1">
         <v>0</v>
@@ -3797,13 +3824,13 @@
         <v>92</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E82" s="1">
         <v>0</v>
@@ -3817,13 +3844,13 @@
         <v>93</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="E83" s="1">
         <v>0</v>
@@ -3846,13 +3873,13 @@
         <v>94</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="E84" s="1">
         <v>1</v>
@@ -3875,13 +3902,13 @@
         <v>95</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="E85" s="1">
         <v>2</v>
@@ -3904,10 +3931,10 @@
         <v>96</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="E86" s="1">
         <v>0</v>
@@ -3919,7 +3946,7 @@
         <v>2</v>
       </c>
       <c r="L86" s="6" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3927,10 +3954,10 @@
         <v>97</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="E87" s="1">
         <v>1</v>
@@ -3942,7 +3969,7 @@
         <v>5</v>
       </c>
       <c r="L87" s="6" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3950,10 +3977,10 @@
         <v>98</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="E88" s="1">
         <v>0</v>
@@ -3962,7 +3989,7 @@
         <v>-10</v>
       </c>
       <c r="L88" s="6" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3970,13 +3997,13 @@
         <v>99</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="E89" s="1">
         <v>1</v>
@@ -3990,13 +4017,13 @@
         <v>100</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="E90" s="1">
         <v>0</v>
@@ -4010,13 +4037,13 @@
         <v>101</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="E91" s="1">
         <v>0</v>
@@ -4030,13 +4057,13 @@
         <v>102</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="E92" s="1">
         <v>0</v>
@@ -4059,13 +4086,13 @@
         <v>103</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>337</v>
+        <v>471</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="E93" s="1">
         <v>1</v>
@@ -4088,13 +4115,13 @@
         <v>104</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="E94" s="1">
         <v>0</v>
@@ -4117,10 +4144,10 @@
         <v>105</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="E95" s="1">
         <v>0</v>
@@ -4137,10 +4164,10 @@
         <v>106</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E96" s="1">
         <v>0</v>
@@ -4154,13 +4181,13 @@
         <v>107</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="E97" s="1">
         <v>0</v>
@@ -4183,13 +4210,13 @@
         <v>108</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="E98" s="1">
         <v>0</v>
@@ -4212,13 +4239,13 @@
         <v>109</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E99" s="1">
         <v>1</v>
@@ -4241,13 +4268,13 @@
         <v>110</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="E100" s="1">
         <v>1</v>
@@ -4270,10 +4297,10 @@
         <v>111</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="E101" s="1">
         <v>0</v>
@@ -4290,10 +4317,10 @@
         <v>112</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="E102" s="1">
         <v>0</v>
@@ -4310,13 +4337,13 @@
         <v>113</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E103" s="1">
         <v>0</v>
@@ -4342,13 +4369,13 @@
         <v>114</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E104" s="1">
         <v>1</v>
@@ -4374,13 +4401,13 @@
         <v>115</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="E105" s="1">
         <v>0</v>
@@ -4391,13 +4418,13 @@
         <v>116</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="E106" s="1">
         <v>2</v>
@@ -4408,13 +4435,13 @@
         <v>117</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="E107" s="1">
         <v>1</v>
@@ -4425,10 +4452,10 @@
         <v>118</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="E108" s="1">
         <v>0</v>
@@ -4439,10 +4466,10 @@
         <v>119</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="E109" s="1">
         <v>0</v>
@@ -4453,10 +4480,10 @@
         <v>120</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="E110" s="1">
         <v>0</v>
@@ -4467,10 +4494,10 @@
         <v>121</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="E111" s="1">
         <v>0</v>
@@ -4481,10 +4508,10 @@
         <v>122</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="E112" s="1">
         <v>0</v>
@@ -4495,10 +4522,10 @@
         <v>123</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="E113" s="1">
         <v>0</v>
@@ -4509,10 +4536,10 @@
         <v>124</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="E114" s="1">
         <v>2</v>
@@ -4523,22 +4550,22 @@
         <v>125</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="E115" s="1">
         <v>1</v>
       </c>
       <c r="L115" s="6" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="M115" s="6" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="N115" s="6" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="O115" s="1">
         <v>1027</v>
@@ -4555,13 +4582,13 @@
         <v>126</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="E116" s="1">
         <v>3</v>
@@ -4572,10 +4599,10 @@
         <v>127</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="E117" s="1">
         <v>0</v>
@@ -4586,10 +4613,10 @@
         <v>128</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="E118" s="1">
         <v>0</v>
@@ -4600,10 +4627,10 @@
         <v>129</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="E119" s="1">
         <v>0</v>
@@ -4614,10 +4641,10 @@
         <v>130</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="E120" s="1">
         <v>0</v>
@@ -4625,13 +4652,13 @@
     </row>
     <row r="121" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="E121" s="1">
         <v>0</v>
@@ -4639,13 +4666,13 @@
     </row>
     <row r="122" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="E122" s="1">
         <v>0</v>
@@ -4653,13 +4680,13 @@
     </row>
     <row r="123" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="E123" s="1">
         <v>0</v>
@@ -4667,13 +4694,13 @@
     </row>
     <row r="124" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="E124" s="1">
         <v>1</v>
@@ -4682,24 +4709,24 @@
         <v>-20</v>
       </c>
       <c r="L124" s="6" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="M124" s="6" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="N124" s="6" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
     </row>
     <row r="125" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="E125" s="1">
         <v>0</v>
@@ -4707,13 +4734,13 @@
     </row>
     <row r="126" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="E126" s="1">
         <v>0</v>
@@ -4721,13 +4748,13 @@
     </row>
     <row r="127" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="E127" s="1">
         <v>0</v>
@@ -4735,13 +4762,13 @@
     </row>
     <row r="128" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="E128" s="1">
         <v>0</v>
@@ -4749,13 +4776,13 @@
     </row>
     <row r="129" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="E129" s="1">
         <v>0</v>
@@ -4763,13 +4790,13 @@
     </row>
     <row r="130" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="E130" s="1">
         <v>2</v>
@@ -4777,27 +4804,27 @@
     </row>
     <row r="131" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="E131" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="E132" s="1">
         <v>0</v>
@@ -4805,15 +4832,57 @@
     </row>
     <row r="133" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="E133" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>1132</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="E134" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>1133</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>1134</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="E133" s="1">
+      <c r="E136" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>